<commit_message>
writeToExcel Hooks a eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\CucumberB6\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="396" windowWidth="17280" windowHeight="8976" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,52 +63,52 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulais1145</t>
-  </si>
-  <si>
-    <t>ulais1146</t>
-  </si>
-  <si>
-    <t>ulais1147</t>
-  </si>
-  <si>
-    <t>ulais1148</t>
-  </si>
-  <si>
-    <t>ulais1149</t>
-  </si>
-  <si>
-    <t>ulais1150</t>
-  </si>
-  <si>
-    <t>ulais1151</t>
-  </si>
-  <si>
-    <t>ulais1152</t>
-  </si>
-  <si>
-    <t>urbs13</t>
-  </si>
-  <si>
-    <t>urbs14</t>
-  </si>
-  <si>
-    <t>urbs15</t>
-  </si>
-  <si>
-    <t>urbs16</t>
-  </si>
-  <si>
-    <t>urbs17</t>
-  </si>
-  <si>
-    <t>urbs18</t>
-  </si>
-  <si>
-    <t>urbs19</t>
-  </si>
-  <si>
-    <t>urbs20</t>
+    <t>urbs134</t>
+  </si>
+  <si>
+    <t>urbs144</t>
+  </si>
+  <si>
+    <t>urbs154</t>
+  </si>
+  <si>
+    <t>urbs164</t>
+  </si>
+  <si>
+    <t>urbs174</t>
+  </si>
+  <si>
+    <t>urbs184</t>
+  </si>
+  <si>
+    <t>urbs194</t>
+  </si>
+  <si>
+    <t>urbs204</t>
+  </si>
+  <si>
+    <t>ul1ais1551</t>
+  </si>
+  <si>
+    <t>ula2is11gg1</t>
+  </si>
+  <si>
+    <t>ulai3s11ff1</t>
+  </si>
+  <si>
+    <t>ulaise114ss1</t>
+  </si>
+  <si>
+    <t>ulaise11xx1</t>
+  </si>
+  <si>
+    <t>ulaeis1vv1</t>
+  </si>
+  <si>
+    <t>ulaifs115bb1</t>
+  </si>
+  <si>
+    <t>ulaisf11ff1</t>
   </si>
 </sst>
 </file>
@@ -433,9 +433,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,7 +465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -481,7 +481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -513,21 +513,21 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -541,13 +541,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -561,13 +561,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -581,13 +581,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -601,13 +601,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -621,13 +621,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -641,13 +641,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -661,12 +661,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>

</xml_diff>